<commit_message>
Feito o orçamento da empresa de Design
</commit_message>
<xml_diff>
--- a/Matérias/Design/Atividades/Projeto Segurança da informação/Informações da Empresa.xlsx
+++ b/Matérias/Design/Atividades/Projeto Segurança da informação/Informações da Empresa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicks\ETEC\Matérias\Design\Atividades\Projeto Segurança da informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B346A21-FD3B-41FA-BBD5-75A4B6C087BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF036D-73DA-400A-BDC8-571942F51639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{60051B29-26A7-43E9-8510-39E3D67571CB}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Funcionários" sheetId="1" r:id="rId1"/>
     <sheet name="Orçamento" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Funcionários!$C$3:$C$31</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,8 +39,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>Nome</t>
   </si>
@@ -268,16 +308,99 @@
   <si>
     <t>Elabora e atualiza o site, cadastra os produtos e controla estoque.</t>
   </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>Valor em Real</t>
+  </si>
+  <si>
+    <t>Valor em Dolar</t>
+  </si>
+  <si>
+    <t>Cotação do Dolar</t>
+  </si>
+  <si>
+    <t>Real para Dolar</t>
+  </si>
+  <si>
+    <t>Equipamentos</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Nome da Empresa</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>Notebook Inspiron 15 3000 SSD 512GB 16GB RAM Placa de vídeo GeForce MX350</t>
+  </si>
+  <si>
+    <t>Dell Technologies</t>
+  </si>
+  <si>
+    <t>Notebook para Designers Web, UX designer e em geral para a área artística da empresa</t>
+  </si>
+  <si>
+    <t>Preço Unidade</t>
+  </si>
+  <si>
+    <t>Preço Total</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Notebook para programadores e as outras áreas da empresa que não neceitam de tanta capacidade de processamento.</t>
+  </si>
+  <si>
+    <t>Custos do Home Office</t>
+  </si>
+  <si>
+    <t>Internet 300 Mb</t>
+  </si>
+  <si>
+    <t>Vivo Internet</t>
+  </si>
+  <si>
+    <t>Cadeira de Escritório Comfy New Stance Plus Tela Mesh Preta, Base Giratória e Sistema Relax</t>
+  </si>
+  <si>
+    <t>Comfy</t>
+  </si>
+  <si>
+    <t>Cadeiras para os funcionários trabalharem em suas casas</t>
+  </si>
+  <si>
+    <t>Custo de Energia</t>
+  </si>
+  <si>
+    <t>Enel</t>
+  </si>
+  <si>
+    <t>Reembolso por energia gasta durante horas de trabalho</t>
+  </si>
+  <si>
+    <t>Notebook Samsung Book Core i5-1135G7, 8G, 256GB SSD, Iris X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +456,25 @@
       <name val="Impact"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -342,7 +484,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -365,12 +507,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -381,11 +705,75 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -402,6 +790,362 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+  <types>
+    <type name="_linkedentity">
+      <keyFlags>
+        <key name="%cvi">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_linkedentitycore">
+      <keyFlags>
+        <key name="%EntityServiceId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntitySubDomainId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityCulture">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%IsRefreshable">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+        <key name="%ProviderInfo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLinkLogo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLink">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%OutdatedReason">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+  </types>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>pt-BR</v>
+    <v>avylgh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Da plataforma Refinitiv</v>
+    <v>0</v>
+    <v>1</v>
+    <v>USD/BRL</v>
+    <v>3</v>
+    <v>4</v>
+    <v>Finance</v>
+    <v>5</v>
+    <v>5.7569999999999997</v>
+    <v>4.5789999999999997</v>
+    <v>5.3021000000000003</v>
+    <v>5.2549000000000001</v>
+    <v>USD</v>
+    <v>5.2530999999999999</v>
+    <v>44823.517222222225</v>
+    <v>BRL</v>
+    <v>US Dollar/Brazilian Real FX Spot Rate</v>
+    <v>5.2538999999999998</v>
+    <v>5.2893999999999997</v>
+    <v>USDBRL</v>
+    <v>Par de Moedas</v>
+    <v>USD/BRL</v>
+    <v>3.6299999999999999E-2</v>
+    <v>6.9099999999999995E-3</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_linkedentitycore">
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="_CanonicalPropertyNames" t="spb"/>
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="52 semanas de alta"/>
+    <k n="52 semanas de baixa"/>
+    <k n="Alto"/>
+    <k n="Baixo"/>
+    <k n="Da moeda" t="s"/>
+    <k n="Fechamento anterior"/>
+    <k n="Hora da última transação"/>
+    <k n="Moeda" t="s"/>
+    <k n="Nome" t="s"/>
+    <k n="Pendência"/>
+    <k n="Preço"/>
+    <k n="Símbolo do ticker" t="s"/>
+    <k n="Tipo de instrumento" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Variação"/>
+    <k n="Variação (%)"/>
+  </s>
+  <s t="_linkedentity">
+    <k n="%cvi" t="r"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
+<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <spbArrays count="1">
+    <a count="28">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">_CanonicalPropertyNames</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Nome</v>
+      <v t="s">Preço</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Hora da última transação</v>
+      <v t="s">Símbolo do ticker</v>
+      <v t="s">Variação</v>
+      <v t="s">Variação (%)</v>
+      <v t="s">Moeda</v>
+      <v t="s">Da moeda</v>
+      <v t="s">Fechamento anterior</v>
+      <v t="s">Pendência</v>
+      <v t="s">Alto</v>
+      <v t="s">Baixo</v>
+      <v t="s">52 semanas de alta</v>
+      <v t="s">52 semanas de baixa</v>
+      <v t="s">Tipo de instrumento</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+  </spbArrays>
+  <spbData count="6">
+    <spb s="0">
+      <v>High</v>
+      <v>Name</v>
+      <v>Low</v>
+      <v>Currency</v>
+      <v>Price</v>
+      <v>From currency</v>
+      <v>Change</v>
+      <v>Open</v>
+      <v>UniqueName</v>
+      <v>Change (%)</v>
+      <v>%ProviderInfo</v>
+      <v>Ticker symbol</v>
+      <v>52 week high</v>
+      <v>52 week low</v>
+      <v>Previous close</v>
+      <v>Instrument type</v>
+      <v>Last trade time</v>
+    </spb>
+    <spb s="1">
+      <v>0</v>
+      <v>Name</v>
+    </spb>
+    <spb s="2">
+      <v>0</v>
+      <v>0</v>
+      <v>0</v>
+    </spb>
+    <spb s="3">
+      <v>2</v>
+      <v>2</v>
+    </spb>
+    <spb s="4">
+      <v>1</v>
+      <v>2</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>3</v>
+      <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
+    </spb>
+    <spb s="5">
+      <v>GMT</v>
+    </spb>
+  </spbData>
+</supportingPropertyBags>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="6">
+  <s>
+    <k n="Alto" t="s"/>
+    <k n="Nome" t="s"/>
+    <k n="Baixo" t="s"/>
+    <k n="Moeda" t="s"/>
+    <k n="Preço" t="s"/>
+    <k n="Da moeda" t="s"/>
+    <k n="Variação" t="s"/>
+    <k n="Pendência" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Variação (%)" t="s"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="Símbolo do ticker" t="s"/>
+    <k n="52 semanas de alta" t="s"/>
+    <k n="52 semanas de baixa" t="s"/>
+    <k n="Fechamento anterior" t="s"/>
+    <k n="Tipo de instrumento" t="s"/>
+    <k n="Hora da última transação" t="s"/>
+  </s>
+  <s>
+    <k n="^Order" t="spba"/>
+    <k n="TitleProperty" t="s"/>
+  </s>
+  <s>
+    <k n="ShowInCardView" t="b"/>
+    <k n="ShowInDotNotation" t="b"/>
+    <k n="ShowInAutoComplete" t="b"/>
+  </s>
+  <s>
+    <k n="UniqueName" t="spb"/>
+    <k n="`%ProviderInfo" t="spb"/>
+  </s>
+  <s>
+    <k n="Alto" t="i"/>
+    <k n="Nome" t="i"/>
+    <k n="Baixo" t="i"/>
+    <k n="Preço" t="i"/>
+    <k n="Variação" t="i"/>
+    <k n="Pendência" t="i"/>
+    <k n="Variação (%)" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="52 semanas de alta" t="i"/>
+    <k n="52 semanas de baixa" t="i"/>
+    <k n="Fechamento anterior" t="i"/>
+    <k n="Hora da última transação" t="i"/>
+  </s>
+  <s>
+    <k n="Hora da última transação" t="s"/>
+  </s>
+</spbStructures>
+</file>
+
+<file path=xl/richData/richStyles.xml><?xml version="1.0" encoding="utf-8"?>
+<richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <dxfs count="4">
+    <x:dxf>
+      <x:numFmt numFmtId="2" formatCode="0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="0" formatCode="General"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="14" formatCode="0.00%"/>
+    </x:dxf>
+  </dxfs>
+  <richProperties>
+    <rPr n="NumberFormat" t="s"/>
+    <rPr n="IsTitleField" t="b"/>
+  </richProperties>
+  <richStyles>
+    <rSty dxfid="1">
+      <rpv i="0">_-[$R$-pt-BR] * #,##0.00_-;-[$R$-pt-BR] * #,##0.00_-;_-[$R$-pt-BR] * "-"??_-;_-@_-</rpv>
+    </rSty>
+    <rSty>
+      <rpv i="1">1</rpv>
+    </rSty>
+    <rSty dxfid="3"/>
+    <rSty dxfid="0">
+      <rpv i="0">0.00</rpv>
+    </rSty>
+    <rSty dxfid="2"/>
+  </richStyles>
+</richStyleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB61FC8-2CBB-46EE-A05B-9C00877F49CE}">
-  <dimension ref="B2:E31"/>
+  <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -714,18 +1458,35 @@
     <col min="3" max="3" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="11" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="1" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="G2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="J2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,8 +1499,21 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="13" cm="1">
+        <f t="array" ref="K3">_FV(J3,"Preço")</f>
+        <v>5.2893999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -749,11 +1523,19 @@
       <c r="D4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>10515.28</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G4" s="18">
+        <f>SUM(E4:E31)</f>
+        <v>175315.28</v>
+      </c>
+      <c r="H4" s="19">
+        <f>PRODUCT(G4,K3)</f>
+        <v>927312.64203199989</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
@@ -763,12 +1545,12 @@
       <c r="D5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>4200</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -777,11 +1559,11 @@
       <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>25000</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -791,11 +1573,11 @@
       <c r="D7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>6700</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -805,11 +1587,11 @@
       <c r="D8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>11200</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -819,11 +1601,11 @@
       <c r="D9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>8200</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -837,7 +1619,7 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -847,11 +1629,11 @@
       <c r="D11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>1700</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="39" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -861,11 +1643,11 @@
       <c r="D12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>4400</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="39" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -875,11 +1657,11 @@
       <c r="D13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>4400</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -889,11 +1671,11 @@
       <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>8500</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -903,11 +1685,11 @@
       <c r="D15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>8500</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
@@ -917,11 +1699,11 @@
       <c r="D16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>8500</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
@@ -931,11 +1713,11 @@
       <c r="D17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>2500</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -945,7 +1727,7 @@
       <c r="D18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>5600</v>
       </c>
     </row>
@@ -959,11 +1741,11 @@
       <c r="D19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>15000</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="39" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -973,7 +1755,7 @@
       <c r="D20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>5200</v>
       </c>
     </row>
@@ -987,11 +1769,11 @@
       <c r="D21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>3800</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="39" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1001,7 +1783,7 @@
       <c r="D22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>4800</v>
       </c>
     </row>
@@ -1015,7 +1797,7 @@
       <c r="D23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>4800</v>
       </c>
     </row>
@@ -1029,7 +1811,7 @@
       <c r="D24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>1600</v>
       </c>
     </row>
@@ -1043,7 +1825,7 @@
       <c r="D25" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>3300</v>
       </c>
     </row>
@@ -1057,7 +1839,7 @@
       <c r="D26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>6200</v>
       </c>
     </row>
@@ -1071,7 +1853,7 @@
       <c r="D27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>3800</v>
       </c>
     </row>
@@ -1085,7 +1867,7 @@
       <c r="D28" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>1700</v>
       </c>
     </row>
@@ -1099,7 +1881,7 @@
       <c r="D29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>1700</v>
       </c>
     </row>
@@ -1113,7 +1895,7 @@
       <c r="D30" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>3800</v>
       </c>
     </row>
@@ -1127,13 +1909,15 @@
       <c r="D31" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>3800</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <autoFilter ref="C3:C31" xr:uid="{DCB61FC8-2CBB-46EE-A05B-9C00877F49CE}"/>
+  <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1142,12 +1926,244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE85F4E0-D8B8-4D67-B646-B1126CC08531}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="G1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+    </row>
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="I2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M3" s="13" cm="1">
+        <f t="array" ref="M3">_FV(L3,"Preço")</f>
+        <v>5.2893999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="34">
+        <v>12</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="25">
+        <v>5617</v>
+      </c>
+      <c r="E4" s="25">
+        <f>PRODUCT(D4,B4)</f>
+        <v>67404</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="18">
+        <f>SUM(E4,E5,E6,E12,E13)</f>
+        <v>162367.72</v>
+      </c>
+      <c r="J4" s="19">
+        <f>PRODUCT(I4,M3)</f>
+        <v>858827.81816799997</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34">
+        <v>16</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="28">
+        <v>3480</v>
+      </c>
+      <c r="E5" s="25">
+        <f>PRODUCT(D5,B5)</f>
+        <v>55680</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="36">
+        <v>28</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="38">
+        <v>1200</v>
+      </c>
+      <c r="E6" s="39">
+        <f>PRODUCT(D6,B6)</f>
+        <v>33600</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B10" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="43">
+        <v>28</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="28">
+        <v>109.99</v>
+      </c>
+      <c r="E12" s="42">
+        <f>PRODUCT(D12,B12)</f>
+        <v>3079.72</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="44"/>
+    </row>
+    <row r="13" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="45">
+        <v>28</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="38">
+        <v>93</v>
+      </c>
+      <c r="E13" s="46">
+        <f>PRODUCT(D13,B13)</f>
+        <v>2604</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Terminado briefing de design EXETO MAPA DE EMPATIA
</commit_message>
<xml_diff>
--- a/Matérias/Design/Atividades/Projeto Segurança da informação/Informações da Empresa.xlsx
+++ b/Matérias/Design/Atividades/Projeto Segurança da informação/Informações da Empresa.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicks\ETEC\Matérias\Design\Atividades\Projeto Segurança da informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF036D-73DA-400A-BDC8-571942F51639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873E255B-5AF2-4245-A00B-61A6CFA4EC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{60051B29-26A7-43E9-8510-39E3D67571CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" activeTab="2" xr2:uid="{60051B29-26A7-43E9-8510-39E3D67571CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionários" sheetId="1" r:id="rId1"/>
     <sheet name="Orçamento" sheetId="2" r:id="rId2"/>
+    <sheet name="Cronograma" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Funcionários!$C$3:$C$31</definedName>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="125">
   <si>
     <t>Nome</t>
   </si>
@@ -389,6 +390,81 @@
   <si>
     <t>Notebook Samsung Book Core i5-1135G7, 8G, 256GB SSD, Iris X</t>
   </si>
+  <si>
+    <t>Tarefas</t>
+  </si>
+  <si>
+    <t>Prazos</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Fev</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Abr</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Ago</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dez</t>
+  </si>
+  <si>
+    <t>Treinamento Design Thinking</t>
+  </si>
+  <si>
+    <t>Treinamento de Trabalho em Grupo</t>
+  </si>
+  <si>
+    <t>Identificação de Riscos</t>
+  </si>
+  <si>
+    <t>Avaliação e tratamento de riscos</t>
+  </si>
+  <si>
+    <t>Medição de Performance</t>
+  </si>
+  <si>
+    <t>Criação Antivirus</t>
+  </si>
+  <si>
+    <t>Criação Aplicação Mobile</t>
+  </si>
+  <si>
+    <t>Criação de VPN</t>
+  </si>
+  <si>
+    <t>Tarefas Realizadas</t>
+  </si>
+  <si>
+    <t>Tarefas a realizar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -397,10 +473,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,13 +551,50 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -694,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -707,9 +820,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -719,22 +829,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -744,15 +848,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -769,11 +864,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -911,20 +1055,20 @@
     <v>5</v>
     <v>5.7569999999999997</v>
     <v>4.5789999999999997</v>
-    <v>5.3021000000000003</v>
-    <v>5.2549000000000001</v>
+    <v>5.1722999999999999</v>
+    <v>5.1680000000000001</v>
     <v>USD</v>
-    <v>5.2530999999999999</v>
-    <v>44823.517222222225</v>
+    <v>5.1669999999999998</v>
+    <v>44824.416898148149</v>
     <v>BRL</v>
     <v>US Dollar/Brazilian Real FX Spot Rate</v>
-    <v>5.2538999999999998</v>
-    <v>5.2893999999999997</v>
+    <v>5.17</v>
+    <v>5.1722999999999999</v>
     <v>USDBRL</v>
     <v>Par de Moedas</v>
     <v>USD/BRL</v>
-    <v>3.6299999999999999E-2</v>
-    <v>6.9099999999999995E-3</v>
+    <v>5.3E-3</v>
+    <v>1.026E-3</v>
   </rv>
   <rv s="1">
     <v>0</v>
@@ -1447,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB61FC8-2CBB-46EE-A05B-9C00877F49CE}">
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:K4"/>
     </sheetView>
   </sheetViews>
@@ -1468,23 +1612,23 @@
   <sheetData>
     <row r="1" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="G2" s="14" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="G2" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="43"/>
+      <c r="J2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -1499,18 +1643,18 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="12" t="e" vm="1">
+      <c r="J3" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K3" s="13" cm="1">
+      <c r="K3" s="12" cm="1">
         <f t="array" ref="K3">_FV(J3,"Preço")</f>
-        <v>5.2893999999999997</v>
+        <v>5.1722999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1526,13 +1670,13 @@
       <c r="E4" s="7">
         <v>10515.28</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="15">
         <f>SUM(E4:E31)</f>
         <v>175315.28</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="16">
         <f>PRODUCT(G4,K3)</f>
-        <v>927312.64203199989</v>
+        <v>906783.22274400003</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
@@ -1759,7 +1903,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1843,7 +1987,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1885,7 +2029,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1899,7 +2043,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="39" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1934,18 +2078,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="18" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="20" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.7109375" customWidth="1"/>
   </cols>
@@ -1959,28 +2103,28 @@
       <c r="N1"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="I2" s="14" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="I2" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1995,111 +2139,111 @@
       <c r="F3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="14" t="s">
         <v>75</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="12" t="e" vm="1">
+      <c r="L3" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="M3" s="13" cm="1">
+      <c r="M3" s="12" cm="1">
         <f t="array" ref="M3">_FV(L3,"Preço")</f>
-        <v>5.2893999999999997</v>
+        <v>5.1722999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34">
+      <c r="B4" s="28">
         <v>12</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>5617</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <f>PRODUCT(D4,B4)</f>
         <v>67404</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="15">
         <f>SUM(E4,E5,E6,E12,E13)</f>
         <v>162367.72</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="16">
         <f>PRODUCT(I4,M3)</f>
-        <v>858827.81816799997</v>
+        <v>839814.55815599998</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34">
+      <c r="B5" s="28">
         <v>16</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="25">
         <v>3480</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
         <f>PRODUCT(D5,B5)</f>
         <v>55680</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="29" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="36">
+      <c r="B6" s="30">
         <v>28</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="32">
         <v>1200</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="33">
         <f>PRODUCT(D6,B6)</f>
         <v>33600</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2114,47 +2258,47 @@
       <c r="F11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="27" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="43">
+      <c r="B12" s="37">
         <v>28</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="25">
         <v>109.99</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="36">
         <f>PRODUCT(D12,B12)</f>
         <v>3079.72</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="38"/>
     </row>
     <row r="13" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="45">
+      <c r="B13" s="39">
         <v>28</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="32">
         <v>93</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="40">
         <f>PRODUCT(D13,B13)</f>
         <v>2604</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="35" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2166,4 +2310,451 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A54187-ADB0-4965-B3ED-091EE1A34F30}">
+  <dimension ref="B1:Z22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="31.5703125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+    </row>
+    <row r="2" spans="2:26" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="54"/>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="55"/>
+      <c r="C3" s="49">
+        <v>2022</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49">
+        <v>2023</v>
+      </c>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="56"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="55"/>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z4" s="57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B5" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="57"/>
+    </row>
+    <row r="6" spans="2:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="57"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="57"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="57"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="57"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="57"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="57"/>
+    </row>
+    <row r="12" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="61"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="63"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="47"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="48"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="8"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="C2:Z2"/>
+  </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>